<commit_message>
Actualización de Matriz de Clases
</commit_message>
<xml_diff>
--- a/Gestion/RIID_MT001.xlsx
+++ b/Gestion/RIID_MT001.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\URP\CICLO 4\Adm Configuracion y Mantenimiento\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18120" windowHeight="6870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18120" windowHeight="6870" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="REQ" sheetId="1" r:id="rId1"/>
+    <sheet name="CLASES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,23 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
-  <si>
-    <t>Paquete: 10 – Administración de Usuario</t>
-  </si>
-  <si>
-    <t>CU.03.01.01 - Logear Usuario.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="42">
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>CU.03.01.02 - Cambiar Contraseña.</t>
-  </si>
-  <si>
-    <t>CU.03.01.03 - Administrar Grupos de Usuario.</t>
-  </si>
-  <si>
     <t>Paquete: 20 – Mantenimiento de Tablas</t>
   </si>
   <si>
@@ -135,12 +119,39 @@
   </si>
   <si>
     <t xml:space="preserve"> X</t>
+  </si>
+  <si>
+    <t>Requisitos vs. Clases</t>
+  </si>
+  <si>
+    <t>FichaController</t>
+  </si>
+  <si>
+    <t>Persona</t>
+  </si>
+  <si>
+    <t>FichaDao</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>ReniecService</t>
+  </si>
+  <si>
+    <t>FichaService</t>
+  </si>
+  <si>
+    <t>DocumentoService</t>
+  </si>
+  <si>
+    <t>DocumentoDao</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -337,7 +348,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -372,7 +383,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -549,7 +560,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -557,49 +568,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="77.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -612,17 +623,25 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -630,42 +649,56 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -674,20 +707,16 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I7" s="4"/>
     </row>
@@ -695,18 +724,16 @@
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I8" s="4"/>
     </row>
@@ -716,15 +743,15 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -733,19 +760,15 @@
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -754,320 +777,529 @@
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="92.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="3.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>